<commit_message>
Complete test with full coverage automate finally
</commit_message>
<xml_diff>
--- a/selenium.automation.framework/src/test/resources/testData.xlsx
+++ b/selenium.automation.framework/src/test/resources/testData.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd62385d097184a9/Desktop/software testing/C4_Project/selenium.automation.framework/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC1048D2695A42EE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4859A69F-9251-40F1-A7ED-3B379484811F}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC1048D2695A42EE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8525F371-4ABA-4490-8B78-8C1426E16552}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registrations" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="Addresses" sheetId="3" r:id="rId3"/>
-    <sheet name="Orders" sheetId="4" r:id="rId4"/>
-    <sheet name="Payments" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="154">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -479,144 +476,6 @@
   </si>
   <si>
     <t>LOGIN-05</t>
-  </si>
-  <si>
-    <t>AddressID</t>
-  </si>
-  <si>
-    <t>UserEmail</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
-  <si>
-    <t>ADDR-01</t>
-  </si>
-  <si>
-    <t>Shipping</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>ADDR-02</t>
-  </si>
-  <si>
-    <t>Billing</t>
-  </si>
-  <si>
-    <t>ADDR-03</t>
-  </si>
-  <si>
-    <t>OrderID</t>
-  </si>
-  <si>
-    <t>ProductID</t>
-  </si>
-  <si>
-    <t>ProductName</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>UnitPrice</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>ORD-1001</t>
-  </si>
-  <si>
-    <t>P-001</t>
-  </si>
-  <si>
-    <t>Blue T-Shirt</t>
-  </si>
-  <si>
-    <t>Placed</t>
-  </si>
-  <si>
-    <t>ORD-1002</t>
-  </si>
-  <si>
-    <t>P-004</t>
-  </si>
-  <si>
-    <t>Red Dress</t>
-  </si>
-  <si>
-    <t>ORD-1003</t>
-  </si>
-  <si>
-    <t>P-010</t>
-  </si>
-  <si>
-    <t>Running Shoes</t>
-  </si>
-  <si>
-    <t>Cancelled</t>
-  </si>
-  <si>
-    <t>PaymentTestID</t>
-  </si>
-  <si>
-    <t>CardName</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>Expiry</t>
-  </si>
-  <si>
-    <t>CVV</t>
-  </si>
-  <si>
-    <t>BillingZip</t>
-  </si>
-  <si>
-    <t>PAY-01</t>
-  </si>
-  <si>
-    <t>12/26</t>
-  </si>
-  <si>
-    <t>Success (Visa test number)</t>
-  </si>
-  <si>
-    <t>PAY-02</t>
-  </si>
-  <si>
-    <t>09/25</t>
-  </si>
-  <si>
-    <t>Fail - card declined (simulated)</t>
-  </si>
-  <si>
-    <t>PAY-03</t>
-  </si>
-  <si>
-    <t>01/27</t>
-  </si>
-  <si>
-    <t>Success (Stripe test number)</t>
-  </si>
-  <si>
-    <t>"4111111111111110"</t>
-  </si>
-  <si>
-    <t>"4000000000000000"</t>
-  </si>
-  <si>
-    <t>"4242424242424240"</t>
   </si>
   <si>
     <t>REG-11</t>
@@ -699,13 +558,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -994,7 +855,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection sqref="A1:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,469 +933,490 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="L7" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>197</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L11" t="s">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="3" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1554,7 +1436,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,7 +1505,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>71</v>
@@ -1637,7 +1519,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>124</v>
@@ -1657,436 +1539,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35C2171-3075-4539-8572-13E00255BD41}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2">
-        <v>90001</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3">
-        <v>400001</v>
-      </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" t="s">
-        <v>132</v>
-      </c>
-      <c r="I4" t="s">
-        <v>131</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4">
-        <v>73301</v>
-      </c>
-      <c r="L4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E521BF-8094-4351-A8DF-BA29163A4CE1}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>45.5</v>
-      </c>
-      <c r="G3">
-        <v>45.5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>79.989999999999995</v>
-      </c>
-      <c r="G4">
-        <v>79.989999999999995</v>
-      </c>
-      <c r="H4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A66F87-864F-4AD1-8D82-4546EF932D0F}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2">
-        <v>123</v>
-      </c>
-      <c r="G2">
-        <v>90001</v>
-      </c>
-      <c r="H2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3">
-        <v>456</v>
-      </c>
-      <c r="G3">
-        <v>400001</v>
-      </c>
-      <c r="H3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4">
-        <v>999</v>
-      </c>
-      <c r="G4">
-        <v>73301</v>
-      </c>
-      <c r="H4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>